<commit_message>
Debagging importDb in FillSheduleService.java, fixed it LessonController.java weekdays/{weekday}
</commit_message>
<xml_diff>
--- a/doc.xlsx
+++ b/doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anton\IdeaProjects\web-service_student_attendance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B81C0B8-0CD1-4DF2-A7F3-2D4072649250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A3745F-33A4-47B1-AA22-FFABB3DFB4DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="150">
   <si>
     <r>
       <rPr>
@@ -407,22 +407,6 @@
         <sz val="12"/>
         <rFont val="Bookman Uralic"/>
       </rPr>
-      <t xml:space="preserve">Проектная деятельность </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Bookman Uralic"/>
-      </rPr>
-      <t>422 М и 426 М преп. Новикова К.Ю.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Bookman Uralic"/>
-      </rPr>
       <t xml:space="preserve">Экономика отрасли </t>
     </r>
     <r>
@@ -530,15 +514,6 @@
         <sz val="12"/>
         <rFont val="Bookman Uralic"/>
       </rPr>
-      <t>530 Г</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Bookman Uralic"/>
-      </rPr>
       <t xml:space="preserve">Иностранный язык в ПД          510 Г
 </t>
     </r>
@@ -1453,15 +1428,6 @@
         <rFont val="Bookman Uralic"/>
       </rPr>
       <t>преп. Костылев С.Ю.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Bookman Uralic"/>
-      </rPr>
-      <t>.</t>
     </r>
   </si>
   <si>
@@ -2558,6 +2524,22 @@
   </si>
   <si>
     <t>СБ</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Bookman Uralic"/>
+      </rPr>
+      <t xml:space="preserve">Проектная деятельность </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Bookman Uralic"/>
+      </rPr>
+      <t>422 М преп. Новикова К.Ю.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2784,7 +2766,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2818,9 +2800,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="5"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2830,20 +2809,23 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2851,11 +2833,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
@@ -2863,16 +2857,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2884,76 +2890,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="23"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="23"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="6"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="6"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="6"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="6"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2971,20 +2920,35 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="6"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="6"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="6"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2997,6 +2961,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3860,7 +3833,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
@@ -3875,70 +3848,70 @@
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" ht="17.7" customHeight="1">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="14" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="D2" s="28" t="s">
-        <v>138</v>
+      <c r="C2" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>135</v>
       </c>
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" ht="16.05" customHeight="1">
-      <c r="A3" s="18"/>
+      <c r="A3" s="25"/>
       <c r="B3" s="21"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" ht="18.75" customHeight="1">
-      <c r="A4" s="18"/>
-      <c r="B4" s="24" t="s">
+      <c r="A4" s="25"/>
+      <c r="B4" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A5" s="18"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A6" s="18"/>
-      <c r="B6" s="24" t="s">
+      <c r="A6" s="25"/>
+      <c r="B6" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A7" s="18"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
+      <c r="A7" s="25"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A8" s="18"/>
-      <c r="B8" s="24" t="s">
+      <c r="A8" s="25"/>
+      <c r="B8" s="28" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="5"/>
@@ -3946,14 +3919,14 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="17.7" customHeight="1">
-      <c r="A9" s="19"/>
-      <c r="B9" s="25"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="29"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" ht="16.8" customHeight="1">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="14" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="20" t="s">
@@ -3964,15 +3937,15 @@
       <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A11" s="18"/>
+      <c r="A11" s="25"/>
       <c r="B11" s="21"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5" ht="17.55" customHeight="1">
-      <c r="A12" s="18"/>
-      <c r="B12" s="24" t="s">
+      <c r="A12" s="25"/>
+      <c r="B12" s="28" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="5"/>
@@ -3980,15 +3953,15 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A13" s="18"/>
-      <c r="B13" s="25"/>
+      <c r="A13" s="25"/>
+      <c r="B13" s="29"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5" ht="18.75" customHeight="1">
-      <c r="A14" s="18"/>
-      <c r="B14" s="24" t="s">
+      <c r="A14" s="25"/>
+      <c r="B14" s="28" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="5"/>
@@ -3996,15 +3969,15 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" ht="18.75" customHeight="1">
-      <c r="A15" s="18"/>
-      <c r="B15" s="25"/>
+      <c r="A15" s="25"/>
+      <c r="B15" s="29"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A16" s="18"/>
-      <c r="B16" s="24" t="s">
+      <c r="A16" s="25"/>
+      <c r="B16" s="28" t="s">
         <v>10</v>
       </c>
       <c r="C16" s="5"/>
@@ -4012,15 +3985,15 @@
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A17" s="18"/>
-      <c r="B17" s="25"/>
+      <c r="A17" s="25"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A18" s="18"/>
-      <c r="B18" s="24" t="s">
+      <c r="A18" s="25"/>
+      <c r="B18" s="28" t="s">
         <v>12</v>
       </c>
       <c r="C18" s="5"/>
@@ -4028,15 +4001,15 @@
       <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:5" ht="17.7" customHeight="1">
-      <c r="A19" s="19"/>
-      <c r="B19" s="25"/>
+      <c r="A19" s="15"/>
+      <c r="B19" s="29"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:5" ht="19.95" customHeight="1">
-      <c r="A20" s="30" t="s">
-        <v>28</v>
+      <c r="A20" s="38" t="s">
+        <v>27</v>
       </c>
       <c r="B20" s="20" t="s">
         <v>5</v>
@@ -4046,15 +4019,15 @@
       <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A21" s="31"/>
+      <c r="A21" s="39"/>
       <c r="B21" s="21"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:5" ht="18.75" customHeight="1">
-      <c r="A22" s="31"/>
-      <c r="B22" s="24" t="s">
+      <c r="A22" s="39"/>
+      <c r="B22" s="28" t="s">
         <v>6</v>
       </c>
       <c r="C22" s="5"/>
@@ -4062,75 +4035,75 @@
       <c r="E22" s="5"/>
     </row>
     <row r="23" spans="1:5" ht="33" customHeight="1">
-      <c r="A23" s="31"/>
-      <c r="B23" s="25"/>
+      <c r="A23" s="39"/>
+      <c r="B23" s="29"/>
       <c r="C23" s="7"/>
       <c r="D23" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E23" s="7"/>
     </row>
     <row r="24" spans="1:5" ht="19.8" customHeight="1">
-      <c r="A24" s="31"/>
-      <c r="B24" s="24" t="s">
+      <c r="A24" s="39"/>
+      <c r="B24" s="28" t="s">
         <v>8</v>
       </c>
       <c r="C24" s="65" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D24" s="66"/>
       <c r="E24" s="5"/>
     </row>
     <row r="25" spans="1:5" ht="33" customHeight="1">
-      <c r="A25" s="31"/>
-      <c r="B25" s="25"/>
+      <c r="A25" s="39"/>
+      <c r="B25" s="29"/>
       <c r="C25" s="7"/>
       <c r="D25" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E25" s="7"/>
+    </row>
+    <row r="26" spans="1:5" ht="16.95" customHeight="1">
+      <c r="A26" s="39"/>
+      <c r="B26" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="61" t="s">
+        <v>139</v>
+      </c>
+      <c r="D26" s="62"/>
+      <c r="E26" s="5"/>
+    </row>
+    <row r="27" spans="1:5" ht="16.95" customHeight="1">
+      <c r="A27" s="39"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="63"/>
+      <c r="D27" s="64"/>
+      <c r="E27" s="5"/>
+    </row>
+    <row r="28" spans="1:5" ht="16.95" customHeight="1">
+      <c r="A28" s="39"/>
+      <c r="B28" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="E28" s="5"/>
+    </row>
+    <row r="29" spans="1:5" ht="33" customHeight="1">
+      <c r="A29" s="40"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="E25" s="7"/>
-    </row>
-    <row r="26" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A26" s="31"/>
-      <c r="B26" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" s="67" t="s">
-        <v>142</v>
-      </c>
-      <c r="D26" s="68"/>
-      <c r="E26" s="5"/>
-    </row>
-    <row r="27" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A27" s="31"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="69"/>
-      <c r="D27" s="70"/>
-      <c r="E27" s="5"/>
-    </row>
-    <row r="28" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A28" s="31"/>
-      <c r="B28" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="28" t="s">
-        <v>143</v>
-      </c>
-      <c r="E28" s="5"/>
-    </row>
-    <row r="29" spans="1:5" ht="33" customHeight="1">
-      <c r="A29" s="32"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D29" s="29"/>
+      <c r="D29" s="31"/>
       <c r="E29" s="7"/>
     </row>
     <row r="30" spans="1:5" ht="19.95" customHeight="1">
-      <c r="A30" s="30" t="s">
-        <v>43</v>
+      <c r="A30" s="38" t="s">
+        <v>41</v>
       </c>
       <c r="B30" s="20" t="s">
         <v>5</v>
@@ -4140,89 +4113,89 @@
       <c r="E30" s="5"/>
     </row>
     <row r="31" spans="1:5" ht="19.2" customHeight="1">
-      <c r="A31" s="31"/>
+      <c r="A31" s="39"/>
       <c r="B31" s="21"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
     </row>
     <row r="32" spans="1:5" ht="33" customHeight="1">
-      <c r="A32" s="31"/>
-      <c r="B32" s="24" t="s">
+      <c r="A32" s="39"/>
+      <c r="B32" s="28" t="s">
         <v>6</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
     </row>
     <row r="33" spans="1:5" ht="33" customHeight="1">
-      <c r="A33" s="31"/>
-      <c r="B33" s="25"/>
+      <c r="A33" s="39"/>
+      <c r="B33" s="29"/>
       <c r="C33" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
     </row>
     <row r="34" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A34" s="31"/>
-      <c r="B34" s="24" t="s">
+      <c r="A34" s="39"/>
+      <c r="B34" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C34" s="28" t="s">
-        <v>143</v>
+      <c r="C34" s="30" t="s">
+        <v>140</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
     </row>
     <row r="35" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A35" s="31"/>
-      <c r="B35" s="25"/>
-      <c r="C35" s="29"/>
+      <c r="A35" s="39"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="31"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
     </row>
     <row r="36" spans="1:5" ht="16.05" customHeight="1">
-      <c r="A36" s="31"/>
-      <c r="B36" s="24" t="s">
+      <c r="A36" s="39"/>
+      <c r="B36" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C36" s="53" t="s">
-        <v>53</v>
-      </c>
-      <c r="D36" s="54"/>
+      <c r="C36" s="51" t="s">
+        <v>51</v>
+      </c>
+      <c r="D36" s="52"/>
       <c r="E36" s="5"/>
     </row>
     <row r="37" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A37" s="31"/>
-      <c r="B37" s="25"/>
-      <c r="C37" s="55"/>
-      <c r="D37" s="56"/>
+      <c r="A37" s="39"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="53"/>
+      <c r="D37" s="54"/>
       <c r="E37" s="5"/>
     </row>
     <row r="38" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A38" s="31"/>
-      <c r="B38" s="24" t="s">
+      <c r="A38" s="39"/>
+      <c r="B38" s="28" t="s">
         <v>12</v>
       </c>
       <c r="C38" s="5"/>
-      <c r="D38" s="28" t="s">
-        <v>143</v>
+      <c r="D38" s="30" t="s">
+        <v>140</v>
       </c>
       <c r="E38" s="5"/>
     </row>
     <row r="39" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A39" s="31"/>
-      <c r="B39" s="25"/>
+      <c r="A39" s="39"/>
+      <c r="B39" s="29"/>
       <c r="C39" s="5"/>
-      <c r="D39" s="29"/>
+      <c r="D39" s="31"/>
       <c r="E39" s="5"/>
     </row>
     <row r="40" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A40" s="31"/>
-      <c r="B40" s="24" t="s">
+      <c r="A40" s="39"/>
+      <c r="B40" s="28" t="s">
         <v>14</v>
       </c>
       <c r="C40" s="5"/>
@@ -4230,15 +4203,15 @@
       <c r="E40" s="5"/>
     </row>
     <row r="41" spans="1:5" ht="17.7" customHeight="1">
-      <c r="A41" s="32"/>
-      <c r="B41" s="25"/>
+      <c r="A41" s="40"/>
+      <c r="B41" s="29"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
     </row>
     <row r="42" spans="1:5" ht="18" customHeight="1">
-      <c r="A42" s="17" t="s">
-        <v>54</v>
+      <c r="A42" s="14" t="s">
+        <v>52</v>
       </c>
       <c r="B42" s="20" t="s">
         <v>5</v>
@@ -4248,15 +4221,15 @@
       <c r="E42" s="5"/>
     </row>
     <row r="43" spans="1:5" ht="22.95" customHeight="1">
-      <c r="A43" s="18"/>
+      <c r="A43" s="25"/>
       <c r="B43" s="21"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
     </row>
     <row r="44" spans="1:5" ht="18.75" customHeight="1">
-      <c r="A44" s="18"/>
-      <c r="B44" s="24" t="s">
+      <c r="A44" s="25"/>
+      <c r="B44" s="28" t="s">
         <v>6</v>
       </c>
       <c r="C44" s="5"/>
@@ -4264,85 +4237,85 @@
       <c r="E44" s="5"/>
     </row>
     <row r="45" spans="1:5" ht="33" customHeight="1">
-      <c r="A45" s="18"/>
-      <c r="B45" s="25"/>
+      <c r="A45" s="25"/>
+      <c r="B45" s="29"/>
       <c r="C45" s="7"/>
       <c r="D45" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E45" s="7"/>
     </row>
     <row r="46" spans="1:5" ht="19.05" customHeight="1">
-      <c r="A46" s="18"/>
-      <c r="B46" s="24" t="s">
+      <c r="A46" s="25"/>
+      <c r="B46" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C46" s="28" t="s">
-        <v>148</v>
-      </c>
-      <c r="D46" s="28" t="s">
-        <v>72</v>
+      <c r="C46" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="D46" s="30" t="s">
+        <v>70</v>
       </c>
       <c r="E46" s="5"/>
     </row>
     <row r="47" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A47" s="18"/>
-      <c r="B47" s="25"/>
-      <c r="C47" s="29"/>
-      <c r="D47" s="29"/>
+      <c r="A47" s="25"/>
+      <c r="B47" s="29"/>
+      <c r="C47" s="31"/>
+      <c r="D47" s="31"/>
       <c r="E47" s="5"/>
     </row>
     <row r="48" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A48" s="18"/>
-      <c r="B48" s="24" t="s">
+      <c r="A48" s="25"/>
+      <c r="B48" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C48" s="67" t="s">
-        <v>142</v>
-      </c>
-      <c r="D48" s="68"/>
+      <c r="C48" s="61" t="s">
+        <v>139</v>
+      </c>
+      <c r="D48" s="62"/>
       <c r="E48" s="5"/>
     </row>
     <row r="49" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A49" s="18"/>
-      <c r="B49" s="25"/>
-      <c r="C49" s="69"/>
-      <c r="D49" s="70"/>
+      <c r="A49" s="25"/>
+      <c r="B49" s="29"/>
+      <c r="C49" s="63"/>
+      <c r="D49" s="64"/>
       <c r="E49" s="5"/>
     </row>
     <row r="50" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A50" s="18"/>
-      <c r="B50" s="24" t="s">
+      <c r="A50" s="25"/>
+      <c r="B50" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C50" s="28" t="s">
-        <v>143</v>
+      <c r="C50" s="30" t="s">
+        <v>140</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
     </row>
     <row r="51" spans="1:5" ht="17.7" customHeight="1">
-      <c r="A51" s="19"/>
-      <c r="B51" s="25"/>
-      <c r="C51" s="29"/>
+      <c r="A51" s="15"/>
+      <c r="B51" s="29"/>
+      <c r="C51" s="31"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
     </row>
     <row r="52" spans="1:5" ht="26.25" customHeight="1">
-      <c r="A52" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="B52" s="13" t="s">
-        <v>59</v>
+      <c r="A52" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
       <c r="E52" s="7"/>
     </row>
     <row r="53" spans="1:5" ht="28.95" customHeight="1">
-      <c r="A53" s="19"/>
-      <c r="B53" s="13" t="s">
-        <v>60</v>
+      <c r="A53" s="15"/>
+      <c r="B53" s="12" t="s">
+        <v>58</v>
       </c>
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
@@ -4350,6 +4323,38 @@
     </row>
   </sheetData>
   <mergeCells count="43">
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C7"/>
+    <mergeCell ref="D2:D7"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A10:A19"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="A20:A29"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:D27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="A30:A41"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:D37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="B40:B41"/>
     <mergeCell ref="A52:A53"/>
     <mergeCell ref="D46:D47"/>
     <mergeCell ref="B48:B49"/>
@@ -4361,38 +4366,6 @@
     <mergeCell ref="B44:B45"/>
     <mergeCell ref="B46:B47"/>
     <mergeCell ref="C46:C47"/>
-    <mergeCell ref="A30:A41"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:D37"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="A20:A29"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:D27"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="A10:A19"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C7"/>
-    <mergeCell ref="D2:D7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4404,7 +4377,7 @@
   <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -4425,13 +4398,13 @@
       <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="16"/>
+      <c r="F1" s="45"/>
     </row>
     <row r="2" spans="1:6" ht="12" customHeight="1">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="14" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="20" t="s">
@@ -4439,30 +4412,30 @@
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="23"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="17"/>
     </row>
     <row r="3" spans="1:6" ht="11.25" customHeight="1">
-      <c r="A3" s="18"/>
+      <c r="A3" s="25"/>
       <c r="B3" s="21"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="23"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="17"/>
     </row>
     <row r="4" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A4" s="18"/>
-      <c r="B4" s="24" t="s">
+      <c r="A4" s="25"/>
+      <c r="B4" s="28" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="23"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="17"/>
     </row>
     <row r="5" spans="1:6" ht="33" customHeight="1">
-      <c r="A5" s="18"/>
-      <c r="B5" s="25"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="29"/>
       <c r="C5" s="7"/>
       <c r="D5" s="2" t="s">
         <v>7</v>
@@ -4471,85 +4444,85 @@
       <c r="F5" s="27"/>
     </row>
     <row r="6" spans="1:6" ht="16.95" customHeight="1">
-      <c r="A6" s="18"/>
-      <c r="B6" s="24" t="s">
+      <c r="A6" s="25"/>
+      <c r="B6" s="28" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="5"/>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="22"/>
-      <c r="F6" s="23"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="17"/>
     </row>
     <row r="7" spans="1:6" ht="16.05" customHeight="1">
-      <c r="A7" s="18"/>
-      <c r="B7" s="25"/>
+      <c r="A7" s="25"/>
+      <c r="B7" s="29"/>
       <c r="C7" s="5"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="23"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="17"/>
     </row>
     <row r="8" spans="1:6" ht="16.95" customHeight="1">
-      <c r="A8" s="18"/>
-      <c r="B8" s="24" t="s">
+      <c r="A8" s="25"/>
+      <c r="B8" s="28" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="5"/>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="22"/>
-      <c r="F8" s="23"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="17"/>
     </row>
     <row r="9" spans="1:6" ht="16.05" customHeight="1">
-      <c r="A9" s="18"/>
-      <c r="B9" s="25"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="29"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="23"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="17"/>
     </row>
     <row r="10" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A10" s="18"/>
-      <c r="B10" s="24" t="s">
+      <c r="A10" s="25"/>
+      <c r="B10" s="28" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="5"/>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="22"/>
-      <c r="F10" s="23"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="17"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A11" s="18"/>
-      <c r="B11" s="25"/>
+      <c r="A11" s="25"/>
+      <c r="B11" s="29"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="23"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="17"/>
     </row>
     <row r="12" spans="1:6" ht="10.95" customHeight="1">
-      <c r="A12" s="18"/>
-      <c r="B12" s="24" t="s">
+      <c r="A12" s="25"/>
+      <c r="B12" s="28" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="23"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="17"/>
     </row>
     <row r="13" spans="1:6" ht="12" customHeight="1">
-      <c r="A13" s="19"/>
-      <c r="B13" s="25"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="29"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="23"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="17"/>
     </row>
     <row r="14" spans="1:6" ht="17.7" customHeight="1">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="38" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="20" t="s">
@@ -4557,11 +4530,11 @@
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="23"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="17"/>
     </row>
     <row r="15" spans="1:6" ht="33" customHeight="1">
-      <c r="A15" s="31"/>
+      <c r="A15" s="39"/>
       <c r="B15" s="21"/>
       <c r="C15" s="7"/>
       <c r="D15" s="2" t="s">
@@ -4575,24 +4548,24 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="33" customHeight="1">
-      <c r="A16" s="31"/>
-      <c r="B16" s="24" t="s">
+      <c r="A16" s="39"/>
+      <c r="B16" s="28" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D16" s="7"/>
-      <c r="E16" s="33" t="s">
+      <c r="E16" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="F16" s="35" t="s">
+      <c r="F16" s="41" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="48.75" customHeight="1">
-      <c r="A17" s="31"/>
-      <c r="B17" s="25"/>
+      <c r="A17" s="39"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="2" t="s">
         <v>22</v>
       </c>
@@ -4600,408 +4573,474 @@
         <v>23</v>
       </c>
       <c r="E17" s="34"/>
-      <c r="F17" s="36"/>
+      <c r="F17" s="42"/>
     </row>
     <row r="18" spans="1:6" ht="33" customHeight="1">
-      <c r="A18" s="31"/>
-      <c r="B18" s="24" t="s">
+      <c r="A18" s="39"/>
+      <c r="B18" s="28" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D18" s="7"/>
-      <c r="E18" s="37" t="s">
+      <c r="E18" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="F18" s="44"/>
+    </row>
+    <row r="19" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A19" s="39"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="38"/>
-    </row>
-    <row r="19" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A19" s="31"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="23"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="17"/>
     </row>
     <row r="20" spans="1:6" ht="28.8" customHeight="1">
-      <c r="A20" s="31"/>
-      <c r="B20" s="24" t="s">
+      <c r="A20" s="39"/>
+      <c r="B20" s="28" t="s">
         <v>10</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="7"/>
-      <c r="E20" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="F20" s="38"/>
+      <c r="E20" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="F20" s="44"/>
     </row>
     <row r="21" spans="1:6" ht="33" customHeight="1">
-      <c r="A21" s="31"/>
-      <c r="B21" s="25"/>
+      <c r="A21" s="39"/>
+      <c r="B21" s="29"/>
       <c r="C21" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="26"/>
       <c r="F21" s="27"/>
     </row>
     <row r="22" spans="1:6" ht="16.95" customHeight="1">
-      <c r="A22" s="31"/>
-      <c r="B22" s="24" t="s">
+      <c r="A22" s="39"/>
+      <c r="B22" s="28" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="23"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="17"/>
     </row>
     <row r="23" spans="1:6" ht="16.8" customHeight="1">
-      <c r="A23" s="32"/>
-      <c r="B23" s="25"/>
+      <c r="A23" s="40"/>
+      <c r="B23" s="29"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="23"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="17"/>
     </row>
     <row r="24" spans="1:6" ht="33" customHeight="1">
-      <c r="A24" s="30" t="s">
-        <v>28</v>
+      <c r="A24" s="38" t="s">
+        <v>27</v>
       </c>
       <c r="B24" s="20" t="s">
         <v>5</v>
       </c>
       <c r="C24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="E24" s="26"/>
       <c r="F24" s="27"/>
     </row>
     <row r="25" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A25" s="31"/>
+      <c r="A25" s="39"/>
       <c r="B25" s="21"/>
-      <c r="C25" s="39" t="s">
+      <c r="C25" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="6"/>
+    </row>
+    <row r="26" spans="1:6" ht="33" customHeight="1">
+      <c r="A26" s="39"/>
+      <c r="B26" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="40"/>
-      <c r="E25" s="11" t="s">
+      <c r="D26" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="F25" s="6"/>
-    </row>
-    <row r="26" spans="1:6" ht="33" customHeight="1">
-      <c r="A26" s="31"/>
-      <c r="B26" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" s="28" t="s">
+      <c r="E26" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D26" s="28" t="s">
+      <c r="F26" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E26" s="8" t="s">
+    </row>
+    <row r="27" spans="1:6" ht="33" customHeight="1">
+      <c r="A27" s="39"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F26" s="12" t="s">
+      <c r="F27" s="9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="33" customHeight="1">
-      <c r="A27" s="31"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F27" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
     <row r="28" spans="1:6" ht="33" customHeight="1">
-      <c r="A28" s="31"/>
+      <c r="A28" s="39"/>
       <c r="B28" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="D28" s="48"/>
-      <c r="E28" s="48"/>
+      <c r="C28" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
       <c r="F28" s="9"/>
     </row>
     <row r="29" spans="1:6" ht="20.25" customHeight="1">
-      <c r="A29" s="31"/>
+      <c r="A29" s="39"/>
       <c r="B29" s="21"/>
-      <c r="C29" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="D29" s="48"/>
-      <c r="E29" s="48"/>
+      <c r="C29" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
       <c r="F29" s="6"/>
     </row>
     <row r="30" spans="1:6" ht="33" customHeight="1">
-      <c r="A30" s="31"/>
-      <c r="B30" s="24" t="s">
+      <c r="A30" s="39"/>
+      <c r="B30" s="28" t="s">
         <v>10</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E30" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="F30" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="E30" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="F30" s="41" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="33" customHeight="1">
-      <c r="A31" s="31"/>
-      <c r="B31" s="25"/>
+      <c r="A31" s="39"/>
+      <c r="B31" s="29"/>
       <c r="C31" s="7"/>
       <c r="D31" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E31" s="34"/>
-      <c r="F31" s="36"/>
+      <c r="F31" s="42"/>
     </row>
     <row r="32" spans="1:6" ht="33" customHeight="1">
-      <c r="A32" s="31"/>
-      <c r="B32" s="24" t="s">
+      <c r="A32" s="39"/>
+      <c r="B32" s="28" t="s">
         <v>12</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F32" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A33" s="32"/>
-      <c r="B33" s="25"/>
+      <c r="A33" s="40"/>
+      <c r="B33" s="29"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="23"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="17"/>
     </row>
     <row r="34" spans="1:6" ht="20.25" customHeight="1">
-      <c r="A34" s="17" t="s">
-        <v>43</v>
+      <c r="A34" s="14" t="s">
+        <v>41</v>
       </c>
       <c r="B34" s="20" t="s">
         <v>5</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
-      <c r="E34" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="F34" s="41"/>
+      <c r="E34" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="F34" s="33"/>
     </row>
     <row r="35" spans="1:6" ht="41.7" customHeight="1">
-      <c r="A35" s="18"/>
+      <c r="A35" s="25"/>
       <c r="B35" s="21"/>
       <c r="C35" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D35" s="7"/>
       <c r="E35" s="34"/>
-      <c r="F35" s="42"/>
+      <c r="F35" s="35"/>
     </row>
     <row r="36" spans="1:6" ht="33" customHeight="1">
-      <c r="A36" s="18"/>
-      <c r="B36" s="24" t="s">
+      <c r="A36" s="25"/>
+      <c r="B36" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C36" s="28" t="s">
-        <v>46</v>
+      <c r="C36" s="30" t="s">
+        <v>44</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E36" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="F36" s="43" t="s">
-        <v>36</v>
+        <v>45</v>
+      </c>
+      <c r="E36" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="F36" s="36" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="16.05" customHeight="1">
-      <c r="A37" s="18"/>
-      <c r="B37" s="25"/>
-      <c r="C37" s="29"/>
+      <c r="A37" s="25"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="31"/>
       <c r="D37" s="5"/>
       <c r="E37" s="34"/>
-      <c r="F37" s="44"/>
+      <c r="F37" s="37"/>
     </row>
     <row r="38" spans="1:6" ht="33" customHeight="1">
-      <c r="A38" s="18"/>
-      <c r="B38" s="24" t="s">
+      <c r="A38" s="25"/>
+      <c r="B38" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C38" s="28" t="s">
+      <c r="C38" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E38" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="F38" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="33" customHeight="1">
+      <c r="A39" s="25"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E38" s="8" t="s">
+      <c r="E39" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F39" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="F38" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="33" customHeight="1">
-      <c r="A39" s="18"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="29"/>
-      <c r="D39" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E39" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F39" s="12" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="40" spans="1:6" ht="33" customHeight="1">
-      <c r="A40" s="18"/>
+      <c r="A40" s="25"/>
       <c r="B40" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C40" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="D40" s="46"/>
-      <c r="E40" s="46"/>
-      <c r="F40" s="47"/>
+      <c r="C40" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="24"/>
     </row>
     <row r="41" spans="1:6" ht="20.25" customHeight="1">
-      <c r="A41" s="18"/>
+      <c r="A41" s="25"/>
       <c r="B41" s="21"/>
-      <c r="C41" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="D41" s="46"/>
-      <c r="E41" s="46"/>
-      <c r="F41" s="47"/>
+      <c r="C41" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D41" s="23"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="24"/>
     </row>
     <row r="42" spans="1:6" ht="11.25" customHeight="1">
-      <c r="A42" s="18"/>
-      <c r="B42" s="24" t="s">
+      <c r="A42" s="25"/>
+      <c r="B42" s="28" t="s">
         <v>12</v>
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="23"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="17"/>
     </row>
     <row r="43" spans="1:6" ht="11.7" customHeight="1">
-      <c r="A43" s="19"/>
-      <c r="B43" s="25"/>
+      <c r="A43" s="15"/>
+      <c r="B43" s="29"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
-      <c r="E43" s="22"/>
-      <c r="F43" s="23"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="17"/>
     </row>
     <row r="44" spans="1:6" ht="18" customHeight="1">
-      <c r="A44" s="17" t="s">
-        <v>54</v>
+      <c r="A44" s="14" t="s">
+        <v>52</v>
       </c>
       <c r="B44" s="20" t="s">
         <v>5</v>
       </c>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
-      <c r="E44" s="22"/>
-      <c r="F44" s="23"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="17"/>
     </row>
     <row r="45" spans="1:6" ht="33" customHeight="1">
-      <c r="A45" s="18"/>
+      <c r="A45" s="25"/>
       <c r="B45" s="21"/>
       <c r="C45" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D45" s="7"/>
       <c r="E45" s="26"/>
       <c r="F45" s="27"/>
     </row>
     <row r="46" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A46" s="18"/>
-      <c r="B46" s="24" t="s">
+      <c r="A46" s="25"/>
+      <c r="B46" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C46" s="28" t="s">
+      <c r="C46" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="D46" s="5"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="17"/>
+    </row>
+    <row r="47" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A47" s="25"/>
+      <c r="B47" s="29"/>
+      <c r="C47" s="31"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="17"/>
+    </row>
+    <row r="48" spans="1:6" ht="24" customHeight="1">
+      <c r="A48" s="25"/>
+      <c r="B48" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="D48" s="5"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="17"/>
+    </row>
+    <row r="49" spans="1:6" ht="24.75" customHeight="1">
+      <c r="A49" s="15"/>
+      <c r="B49" s="29"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="17"/>
+    </row>
+    <row r="50" spans="1:6" ht="22.05" customHeight="1">
+      <c r="A50" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="D46" s="5"/>
-      <c r="E46" s="22"/>
-      <c r="F46" s="23"/>
-    </row>
-    <row r="47" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A47" s="18"/>
-      <c r="B47" s="25"/>
-      <c r="C47" s="29"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="22"/>
-      <c r="F47" s="23"/>
-    </row>
-    <row r="48" spans="1:6" ht="24" customHeight="1">
-      <c r="A48" s="18"/>
-      <c r="B48" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="C48" s="28" t="s">
+      <c r="B50" s="12" t="s">
         <v>57</v>
-      </c>
-      <c r="D48" s="5"/>
-      <c r="E48" s="22"/>
-      <c r="F48" s="23"/>
-    </row>
-    <row r="49" spans="1:6" ht="24.75" customHeight="1">
-      <c r="A49" s="19"/>
-      <c r="B49" s="25"/>
-      <c r="C49" s="29"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="22"/>
-      <c r="F49" s="23"/>
-    </row>
-    <row r="50" spans="1:6" ht="22.05" customHeight="1">
-      <c r="A50" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="B50" s="13" t="s">
-        <v>59</v>
       </c>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
-      <c r="E50" s="22"/>
-      <c r="F50" s="23"/>
+      <c r="E50" s="16"/>
+      <c r="F50" s="17"/>
     </row>
     <row r="51" spans="1:6" ht="17.7" customHeight="1">
-      <c r="A51" s="19"/>
-      <c r="B51" s="13" t="s">
-        <v>60</v>
+      <c r="A51" s="15"/>
+      <c r="B51" s="12" t="s">
+        <v>58</v>
       </c>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
-      <c r="E51" s="22"/>
-      <c r="F51" s="23"/>
+      <c r="E51" s="16"/>
+      <c r="F51" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="84">
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="A14:A23"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="A24:A33"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="A34:A43"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="E34:F35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="C41:F41"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="E42:F42"/>
     <mergeCell ref="A50:A51"/>
     <mergeCell ref="E50:F50"/>
     <mergeCell ref="E51:F51"/>
@@ -5018,74 +5057,6 @@
     <mergeCell ref="C46:C47"/>
     <mergeCell ref="E46:F46"/>
     <mergeCell ref="E47:F47"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="A34:A43"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="E34:F35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="C41:F41"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="A24:A33"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="A14:A23"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5118,7 +5089,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
@@ -5133,15 +5104,15 @@
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" ht="10.95" customHeight="1">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="14" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="20" t="s">
@@ -5152,15 +5123,15 @@
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" ht="9.75" customHeight="1">
-      <c r="A3" s="18"/>
+      <c r="A3" s="25"/>
       <c r="B3" s="21"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" ht="10.199999999999999" customHeight="1">
-      <c r="A4" s="18"/>
-      <c r="B4" s="24" t="s">
+      <c r="A4" s="25"/>
+      <c r="B4" s="28" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="5"/>
@@ -5168,15 +5139,15 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" ht="10.050000000000001" customHeight="1">
-      <c r="A5" s="18"/>
-      <c r="B5" s="25"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="29"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" ht="10.199999999999999" customHeight="1">
-      <c r="A6" s="18"/>
-      <c r="B6" s="24" t="s">
+      <c r="A6" s="25"/>
+      <c r="B6" s="28" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="5"/>
@@ -5184,15 +5155,15 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" ht="10.050000000000001" customHeight="1">
-      <c r="A7" s="18"/>
-      <c r="B7" s="25"/>
+      <c r="A7" s="25"/>
+      <c r="B7" s="29"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" ht="21" customHeight="1">
-      <c r="A8" s="18"/>
-      <c r="B8" s="24" t="s">
+      <c r="A8" s="25"/>
+      <c r="B8" s="28" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="5"/>
@@ -5200,15 +5171,15 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A9" s="18"/>
-      <c r="B9" s="25"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="29"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1">
-      <c r="A10" s="18"/>
-      <c r="B10" s="24" t="s">
+      <c r="A10" s="25"/>
+      <c r="B10" s="28" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="5"/>
@@ -5216,14 +5187,14 @@
       <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:5" ht="21.3" customHeight="1">
-      <c r="A11" s="19"/>
-      <c r="B11" s="25"/>
+      <c r="A11" s="15"/>
+      <c r="B11" s="29"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5" ht="16.8" customHeight="1">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="14" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="20" t="s">
@@ -5234,15 +5205,15 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" ht="16.05" customHeight="1">
-      <c r="A13" s="18"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="21"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5" ht="17.55" customHeight="1">
-      <c r="A14" s="18"/>
-      <c r="B14" s="24" t="s">
+      <c r="A14" s="25"/>
+      <c r="B14" s="28" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="5"/>
@@ -5250,15 +5221,15 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A15" s="18"/>
-      <c r="B15" s="25"/>
+      <c r="A15" s="25"/>
+      <c r="B15" s="29"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5" ht="18.75" customHeight="1">
-      <c r="A16" s="18"/>
-      <c r="B16" s="24" t="s">
+      <c r="A16" s="25"/>
+      <c r="B16" s="28" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="5"/>
@@ -5266,17 +5237,17 @@
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="33" customHeight="1">
-      <c r="A17" s="18"/>
-      <c r="B17" s="25"/>
+      <c r="A17" s="25"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
     </row>
     <row r="18" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A18" s="18"/>
-      <c r="B18" s="24" t="s">
+      <c r="A18" s="25"/>
+      <c r="B18" s="28" t="s">
         <v>10</v>
       </c>
       <c r="C18" s="5"/>
@@ -5284,8 +5255,8 @@
       <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:5" ht="33" customHeight="1">
-      <c r="A19" s="18"/>
-      <c r="B19" s="25"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="29"/>
       <c r="C19" s="2" t="s">
         <v>23</v>
       </c>
@@ -5293,8 +5264,8 @@
       <c r="E19" s="7"/>
     </row>
     <row r="20" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A20" s="18"/>
-      <c r="B20" s="24" t="s">
+      <c r="A20" s="25"/>
+      <c r="B20" s="28" t="s">
         <v>12</v>
       </c>
       <c r="C20" s="5"/>
@@ -5302,8 +5273,8 @@
       <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:5" ht="33" customHeight="1">
-      <c r="A21" s="19"/>
-      <c r="B21" s="25"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="29"/>
       <c r="C21" s="2" t="s">
         <v>23</v>
       </c>
@@ -5311,8 +5282,8 @@
       <c r="E21" s="7"/>
     </row>
     <row r="22" spans="1:5" ht="19.95" customHeight="1">
-      <c r="A22" s="30" t="s">
-        <v>28</v>
+      <c r="A22" s="38" t="s">
+        <v>27</v>
       </c>
       <c r="B22" s="20" t="s">
         <v>5</v>
@@ -5322,75 +5293,75 @@
       <c r="E22" s="5"/>
     </row>
     <row r="23" spans="1:5" ht="33" customHeight="1">
-      <c r="A23" s="31"/>
+      <c r="A23" s="39"/>
       <c r="B23" s="21"/>
       <c r="C23" s="7"/>
       <c r="D23" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E23" s="7"/>
     </row>
     <row r="24" spans="1:5" ht="33" customHeight="1">
-      <c r="A24" s="31"/>
-      <c r="B24" s="24" t="s">
+      <c r="A24" s="39"/>
+      <c r="B24" s="28" t="s">
         <v>6</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24" s="7"/>
+    </row>
+    <row r="25" spans="1:5" ht="33" customHeight="1">
+      <c r="A25" s="39"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E24" s="7"/>
-    </row>
-    <row r="25" spans="1:5" ht="33" customHeight="1">
-      <c r="A25" s="31"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="2" t="s">
+      <c r="E25" s="7"/>
+    </row>
+    <row r="26" spans="1:5" ht="10.95" customHeight="1">
+      <c r="A26" s="39"/>
+      <c r="B26" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="55" t="s">
         <v>66</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D26" s="56"/>
+      <c r="E26" s="5"/>
+    </row>
+    <row r="27" spans="1:5" ht="10.95" customHeight="1">
+      <c r="A27" s="39"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="57"/>
+      <c r="D27" s="58"/>
+      <c r="E27" s="5"/>
+    </row>
+    <row r="28" spans="1:5" ht="16.95" customHeight="1">
+      <c r="A28" s="39"/>
+      <c r="B28" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="30" t="s">
         <v>67</v>
-      </c>
-      <c r="E25" s="7"/>
-    </row>
-    <row r="26" spans="1:5" ht="10.95" customHeight="1">
-      <c r="A26" s="31"/>
-      <c r="B26" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="C26" s="49" t="s">
-        <v>68</v>
-      </c>
-      <c r="D26" s="50"/>
-      <c r="E26" s="5"/>
-    </row>
-    <row r="27" spans="1:5" ht="10.95" customHeight="1">
-      <c r="A27" s="31"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="51"/>
-      <c r="D27" s="52"/>
-      <c r="E27" s="5"/>
-    </row>
-    <row r="28" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A28" s="31"/>
-      <c r="B28" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28" s="28" t="s">
-        <v>69</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
     </row>
     <row r="29" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A29" s="31"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="29"/>
+      <c r="A29" s="39"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="31"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
     </row>
     <row r="30" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A30" s="31"/>
-      <c r="B30" s="24" t="s">
+      <c r="A30" s="39"/>
+      <c r="B30" s="28" t="s">
         <v>12</v>
       </c>
       <c r="C30" s="5"/>
@@ -5398,95 +5369,95 @@
       <c r="E30" s="5"/>
     </row>
     <row r="31" spans="1:5" ht="17.7" customHeight="1">
-      <c r="A31" s="32"/>
-      <c r="B31" s="25"/>
+      <c r="A31" s="40"/>
+      <c r="B31" s="29"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
     </row>
     <row r="32" spans="1:5" ht="20.25" customHeight="1">
-      <c r="A32" s="17" t="s">
-        <v>43</v>
+      <c r="A32" s="14" t="s">
+        <v>41</v>
       </c>
       <c r="B32" s="20" t="s">
         <v>5</v>
       </c>
       <c r="C32" s="5"/>
-      <c r="D32" s="28" t="s">
-        <v>70</v>
+      <c r="D32" s="30" t="s">
+        <v>68</v>
       </c>
       <c r="E32" s="5"/>
     </row>
     <row r="33" spans="1:5" ht="19.2" customHeight="1">
-      <c r="A33" s="18"/>
+      <c r="A33" s="25"/>
       <c r="B33" s="21"/>
       <c r="C33" s="5"/>
-      <c r="D33" s="29"/>
+      <c r="D33" s="31"/>
       <c r="E33" s="5"/>
     </row>
     <row r="34" spans="1:5" ht="33" customHeight="1">
-      <c r="A34" s="18"/>
-      <c r="B34" s="24" t="s">
+      <c r="A34" s="25"/>
+      <c r="B34" s="28" t="s">
         <v>6</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D34" s="28" t="s">
+      <c r="D34" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="E34" s="7"/>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A35" s="25"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="5"/>
+    </row>
+    <row r="36" spans="1:5" ht="33" customHeight="1">
+      <c r="A36" s="25"/>
+      <c r="B36" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D36" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="E34" s="7"/>
-    </row>
-    <row r="35" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A35" s="18"/>
-      <c r="B35" s="25"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="5"/>
-    </row>
-    <row r="36" spans="1:5" ht="33" customHeight="1">
-      <c r="A36" s="18"/>
-      <c r="B36" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D36" s="28" t="s">
-        <v>73</v>
-      </c>
       <c r="E36" s="7"/>
     </row>
     <row r="37" spans="1:5" ht="33" customHeight="1">
-      <c r="A37" s="18"/>
-      <c r="B37" s="25"/>
+      <c r="A37" s="25"/>
+      <c r="B37" s="29"/>
       <c r="C37" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D37" s="29"/>
+        <v>67</v>
+      </c>
+      <c r="D37" s="31"/>
       <c r="E37" s="7"/>
     </row>
     <row r="38" spans="1:5" ht="11.25" customHeight="1">
-      <c r="A38" s="18"/>
-      <c r="B38" s="24" t="s">
+      <c r="A38" s="25"/>
+      <c r="B38" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C38" s="53" t="s">
-        <v>53</v>
-      </c>
-      <c r="D38" s="54"/>
+      <c r="C38" s="51" t="s">
+        <v>51</v>
+      </c>
+      <c r="D38" s="52"/>
       <c r="E38" s="5"/>
     </row>
     <row r="39" spans="1:5" ht="10.95" customHeight="1">
-      <c r="A39" s="18"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="55"/>
-      <c r="D39" s="56"/>
+      <c r="A39" s="25"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="53"/>
+      <c r="D39" s="54"/>
       <c r="E39" s="5"/>
     </row>
     <row r="40" spans="1:5" ht="16.05" customHeight="1">
-      <c r="A40" s="18"/>
-      <c r="B40" s="24" t="s">
+      <c r="A40" s="25"/>
+      <c r="B40" s="28" t="s">
         <v>12</v>
       </c>
       <c r="C40" s="5"/>
@@ -5494,53 +5465,53 @@
       <c r="E40" s="5"/>
     </row>
     <row r="41" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A41" s="19"/>
-      <c r="B41" s="25"/>
+      <c r="A41" s="15"/>
+      <c r="B41" s="29"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
     </row>
     <row r="42" spans="1:5" ht="18" customHeight="1">
-      <c r="A42" s="17" t="s">
-        <v>54</v>
+      <c r="A42" s="14" t="s">
+        <v>52</v>
       </c>
       <c r="B42" s="20" t="s">
         <v>5</v>
       </c>
       <c r="C42" s="5"/>
-      <c r="D42" s="28" t="s">
-        <v>74</v>
+      <c r="D42" s="30" t="s">
+        <v>72</v>
       </c>
       <c r="E42" s="5"/>
     </row>
     <row r="43" spans="1:5" ht="22.95" customHeight="1">
-      <c r="A43" s="18"/>
+      <c r="A43" s="25"/>
       <c r="B43" s="21"/>
       <c r="C43" s="5"/>
-      <c r="D43" s="29"/>
+      <c r="D43" s="31"/>
       <c r="E43" s="5"/>
     </row>
     <row r="44" spans="1:5" ht="18.75" customHeight="1">
-      <c r="A44" s="18"/>
-      <c r="B44" s="24" t="s">
+      <c r="A44" s="25"/>
+      <c r="B44" s="28" t="s">
         <v>6</v>
       </c>
       <c r="C44" s="5"/>
-      <c r="D44" s="28" t="s">
-        <v>75</v>
+      <c r="D44" s="30" t="s">
+        <v>73</v>
       </c>
       <c r="E44" s="5"/>
     </row>
     <row r="45" spans="1:5" ht="18.45" customHeight="1">
-      <c r="A45" s="18"/>
-      <c r="B45" s="25"/>
+      <c r="A45" s="25"/>
+      <c r="B45" s="29"/>
       <c r="C45" s="5"/>
-      <c r="D45" s="29"/>
+      <c r="D45" s="31"/>
       <c r="E45" s="5"/>
     </row>
     <row r="46" spans="1:5" ht="11.25" customHeight="1">
-      <c r="A46" s="18"/>
-      <c r="B46" s="24" t="s">
+      <c r="A46" s="25"/>
+      <c r="B46" s="28" t="s">
         <v>8</v>
       </c>
       <c r="C46" s="5"/>
@@ -5548,72 +5519,102 @@
       <c r="E46" s="5"/>
     </row>
     <row r="47" spans="1:5" ht="33" customHeight="1">
-      <c r="A47" s="19"/>
-      <c r="B47" s="25"/>
+      <c r="A47" s="15"/>
+      <c r="B47" s="29"/>
       <c r="C47" s="7"/>
       <c r="D47" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E47" s="7"/>
+    </row>
+    <row r="48" spans="1:5" ht="33" customHeight="1">
+      <c r="A48" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="B48" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" s="30" t="s">
         <v>76</v>
-      </c>
-      <c r="E47" s="7"/>
-    </row>
-    <row r="48" spans="1:5" ht="33" customHeight="1">
-      <c r="A48" s="59" t="s">
-        <v>77</v>
-      </c>
-      <c r="B48" s="57" t="s">
-        <v>5</v>
-      </c>
-      <c r="C48" s="28" t="s">
-        <v>78</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="7"/>
     </row>
     <row r="49" spans="1:5" ht="58.5" customHeight="1">
-      <c r="A49" s="60"/>
-      <c r="B49" s="58"/>
-      <c r="C49" s="29"/>
+      <c r="A49" s="49"/>
+      <c r="B49" s="47"/>
+      <c r="C49" s="31"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
     </row>
     <row r="50" spans="1:5" ht="58.5" customHeight="1">
-      <c r="A50" s="60"/>
-      <c r="B50" s="57" t="s">
+      <c r="A50" s="49"/>
+      <c r="B50" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="C50" s="28" t="s">
-        <v>79</v>
+      <c r="C50" s="30" t="s">
+        <v>77</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
     </row>
     <row r="51" spans="1:5" ht="55.8" customHeight="1">
-      <c r="A51" s="60"/>
-      <c r="B51" s="58"/>
-      <c r="C51" s="29"/>
+      <c r="A51" s="49"/>
+      <c r="B51" s="47"/>
+      <c r="C51" s="31"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
     </row>
     <row r="52" spans="1:5" ht="54.45" customHeight="1">
-      <c r="A52" s="60"/>
-      <c r="B52" s="24" t="s">
+      <c r="A52" s="49"/>
+      <c r="B52" s="28" t="s">
         <v>8</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
     </row>
     <row r="53" spans="1:5" ht="28.95" customHeight="1">
-      <c r="A53" s="61"/>
-      <c r="B53" s="25"/>
+      <c r="A53" s="50"/>
+      <c r="B53" s="29"/>
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
       <c r="E53" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="A2:A11"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A12:A21"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A22:A31"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:D27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="A32:A41"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:D39"/>
+    <mergeCell ref="B40:B41"/>
     <mergeCell ref="B52:B53"/>
     <mergeCell ref="A42:A47"/>
     <mergeCell ref="B42:B43"/>
@@ -5626,36 +5627,6 @@
     <mergeCell ref="C50:C51"/>
     <mergeCell ref="B50:B51"/>
     <mergeCell ref="A48:A53"/>
-    <mergeCell ref="A32:A41"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:D39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="A22:A31"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:D27"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="A12:A21"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A2:A11"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5688,8 +5659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48:A55"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -5703,15 +5674,15 @@
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" ht="12" customHeight="1">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="14" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="20" t="s">
@@ -5722,89 +5693,89 @@
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" ht="11.25" customHeight="1">
-      <c r="A3" s="18"/>
+      <c r="A3" s="25"/>
       <c r="B3" s="21"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" ht="48.75" customHeight="1">
-      <c r="A4" s="18"/>
-      <c r="B4" s="24" t="s">
+      <c r="A4" s="25"/>
+      <c r="B4" s="28" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A5" s="18"/>
-      <c r="B5" s="25"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="29"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" ht="33" customHeight="1">
-      <c r="A6" s="18"/>
-      <c r="B6" s="24" t="s">
+      <c r="A6" s="25"/>
+      <c r="B6" s="28" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" ht="33" customHeight="1">
-      <c r="A7" s="18"/>
-      <c r="B7" s="25"/>
+      <c r="A7" s="25"/>
+      <c r="B7" s="29"/>
       <c r="C7" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:5" ht="22.95" customHeight="1">
-      <c r="A8" s="18"/>
-      <c r="B8" s="24" t="s">
+      <c r="A8" s="25"/>
+      <c r="B8" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="28" t="s">
-        <v>85</v>
+      <c r="C8" s="30" t="s">
+        <v>83</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="25.8" customHeight="1">
-      <c r="A9" s="18"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="29"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="31"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A10" s="18"/>
-      <c r="B10" s="24" t="s">
+      <c r="A10" s="25"/>
+      <c r="B10" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="28" t="s">
-        <v>86</v>
+      <c r="C10" s="30" t="s">
+        <v>84</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A11" s="18"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="29"/>
+      <c r="A11" s="25"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="31"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5" ht="10.95" customHeight="1">
-      <c r="A12" s="18"/>
-      <c r="B12" s="24" t="s">
+      <c r="A12" s="25"/>
+      <c r="B12" s="28" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="5"/>
@@ -5812,59 +5783,59 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" ht="11.7" customHeight="1">
-      <c r="A13" s="19"/>
-      <c r="B13" s="25"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="29"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5" ht="16.8" customHeight="1">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="14" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="28" t="s">
-        <v>83</v>
-      </c>
-      <c r="D14" s="28" t="s">
-        <v>87</v>
+      <c r="C14" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>85</v>
       </c>
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A15" s="18"/>
+      <c r="A15" s="25"/>
       <c r="B15" s="21"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5" ht="33" customHeight="1">
-      <c r="A16" s="18"/>
-      <c r="B16" s="24" t="s">
+      <c r="A16" s="25"/>
+      <c r="B16" s="28" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D16" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>85</v>
       </c>
       <c r="E16" s="7"/>
     </row>
     <row r="17" spans="1:5" ht="33" customHeight="1">
-      <c r="A17" s="18"/>
-      <c r="B17" s="25"/>
+      <c r="A17" s="25"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D17" s="29"/>
+        <v>81</v>
+      </c>
+      <c r="D17" s="31"/>
       <c r="E17" s="7"/>
     </row>
     <row r="18" spans="1:5" ht="10.95" customHeight="1">
-      <c r="A18" s="18"/>
-      <c r="B18" s="24" t="s">
+      <c r="A18" s="25"/>
+      <c r="B18" s="28" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="5"/>
@@ -5872,15 +5843,15 @@
       <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:5" ht="11.7" customHeight="1">
-      <c r="A19" s="19"/>
-      <c r="B19" s="25"/>
+      <c r="A19" s="15"/>
+      <c r="B19" s="29"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:5" ht="12" customHeight="1">
-      <c r="A20" s="30" t="s">
-        <v>28</v>
+      <c r="A20" s="38" t="s">
+        <v>27</v>
       </c>
       <c r="B20" s="20" t="s">
         <v>5</v>
@@ -5890,75 +5861,73 @@
       <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:5" ht="11.25" customHeight="1">
-      <c r="A21" s="31"/>
+      <c r="A21" s="39"/>
       <c r="B21" s="21"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:5" ht="11.25" customHeight="1">
-      <c r="A22" s="31"/>
-      <c r="B22" s="24" t="s">
+      <c r="A22" s="39"/>
+      <c r="B22" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="14" t="s">
-        <v>89</v>
-      </c>
+      <c r="C22" s="13"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
     </row>
     <row r="23" spans="1:5" ht="33" customHeight="1">
-      <c r="A23" s="31"/>
-      <c r="B23" s="25"/>
+      <c r="A23" s="39"/>
+      <c r="B23" s="29"/>
       <c r="C23" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
     </row>
     <row r="24" spans="1:5" ht="33" customHeight="1">
-      <c r="A24" s="31"/>
-      <c r="B24" s="24" t="s">
+      <c r="A24" s="39"/>
+      <c r="B24" s="28" t="s">
         <v>8</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
     </row>
     <row r="25" spans="1:5" ht="33" customHeight="1">
-      <c r="A25" s="31"/>
-      <c r="B25" s="25"/>
+      <c r="A25" s="39"/>
+      <c r="B25" s="29"/>
       <c r="C25" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
     </row>
     <row r="26" spans="1:5" ht="33" customHeight="1">
-      <c r="A26" s="31"/>
-      <c r="B26" s="24" t="s">
+      <c r="A26" s="39"/>
+      <c r="B26" s="28" t="s">
         <v>10</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
     </row>
     <row r="27" spans="1:5" ht="33" customHeight="1">
-      <c r="A27" s="31"/>
-      <c r="B27" s="25"/>
+      <c r="A27" s="39"/>
+      <c r="B27" s="29"/>
       <c r="C27" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
     </row>
     <row r="28" spans="1:5" ht="10.050000000000001" customHeight="1">
-      <c r="A28" s="31"/>
-      <c r="B28" s="24" t="s">
+      <c r="A28" s="39"/>
+      <c r="B28" s="28" t="s">
         <v>12</v>
       </c>
       <c r="C28" s="5"/>
@@ -5966,95 +5935,95 @@
       <c r="E28" s="5"/>
     </row>
     <row r="29" spans="1:5" ht="10.5" customHeight="1">
-      <c r="A29" s="32"/>
-      <c r="B29" s="25"/>
+      <c r="A29" s="40"/>
+      <c r="B29" s="29"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
     </row>
     <row r="30" spans="1:5" ht="48.75" customHeight="1">
-      <c r="A30" s="17" t="s">
-        <v>43</v>
+      <c r="A30" s="14" t="s">
+        <v>41</v>
       </c>
       <c r="B30" s="20" t="s">
         <v>5</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
     </row>
     <row r="31" spans="1:5" ht="33" customHeight="1">
-      <c r="A31" s="18"/>
+      <c r="A31" s="25"/>
       <c r="B31" s="21"/>
       <c r="C31" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
     </row>
     <row r="32" spans="1:5" ht="21.75" customHeight="1">
-      <c r="A32" s="18"/>
-      <c r="B32" s="24" t="s">
+      <c r="A32" s="25"/>
+      <c r="B32" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="D32" s="28" t="s">
-        <v>96</v>
+      <c r="C32" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="D32" s="30" t="s">
+        <v>93</v>
       </c>
       <c r="E32" s="7"/>
     </row>
     <row r="33" spans="1:5" ht="27" customHeight="1">
-      <c r="A33" s="18"/>
-      <c r="B33" s="25"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="29"/>
+      <c r="A33" s="25"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
       <c r="E33" s="7"/>
     </row>
     <row r="34" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A34" s="18"/>
-      <c r="B34" s="24" t="s">
+      <c r="A34" s="25"/>
+      <c r="B34" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C34" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="D34" s="28" t="s">
-        <v>96</v>
+      <c r="C34" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D34" s="30" t="s">
+        <v>93</v>
       </c>
       <c r="E34" s="5"/>
     </row>
     <row r="35" spans="1:5" ht="16.05" customHeight="1">
-      <c r="A35" s="18"/>
-      <c r="B35" s="25"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
+      <c r="A35" s="25"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
       <c r="E35" s="5"/>
     </row>
     <row r="36" spans="1:5" ht="10.95" customHeight="1">
-      <c r="A36" s="18"/>
-      <c r="B36" s="24" t="s">
+      <c r="A36" s="25"/>
+      <c r="B36" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C36" s="53" t="s">
-        <v>53</v>
-      </c>
-      <c r="D36" s="54"/>
+      <c r="C36" s="51" t="s">
+        <v>51</v>
+      </c>
+      <c r="D36" s="52"/>
       <c r="E36" s="5"/>
     </row>
     <row r="37" spans="1:5" ht="11.25" customHeight="1">
-      <c r="A37" s="18"/>
-      <c r="B37" s="25"/>
-      <c r="C37" s="55"/>
-      <c r="D37" s="56"/>
+      <c r="A37" s="25"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="53"/>
+      <c r="D37" s="54"/>
       <c r="E37" s="5"/>
     </row>
     <row r="38" spans="1:5" ht="16.05" customHeight="1">
-      <c r="A38" s="18"/>
-      <c r="B38" s="24" t="s">
+      <c r="A38" s="25"/>
+      <c r="B38" s="28" t="s">
         <v>12</v>
       </c>
       <c r="C38" s="5"/>
@@ -6062,15 +6031,15 @@
       <c r="E38" s="5"/>
     </row>
     <row r="39" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A39" s="19"/>
-      <c r="B39" s="25"/>
+      <c r="A39" s="15"/>
+      <c r="B39" s="29"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
     </row>
     <row r="40" spans="1:5" ht="10.8" customHeight="1">
-      <c r="A40" s="17" t="s">
-        <v>54</v>
+      <c r="A40" s="14" t="s">
+        <v>52</v>
       </c>
       <c r="B40" s="20" t="s">
         <v>5</v>
@@ -6080,15 +6049,15 @@
       <c r="E40" s="5"/>
     </row>
     <row r="41" spans="1:5" ht="11.25" customHeight="1">
-      <c r="A41" s="18"/>
+      <c r="A41" s="25"/>
       <c r="B41" s="21"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
     </row>
     <row r="42" spans="1:5" ht="10.95" customHeight="1">
-      <c r="A42" s="18"/>
-      <c r="B42" s="24" t="s">
+      <c r="A42" s="25"/>
+      <c r="B42" s="28" t="s">
         <v>6</v>
       </c>
       <c r="C42" s="5"/>
@@ -6096,15 +6065,15 @@
       <c r="E42" s="5"/>
     </row>
     <row r="43" spans="1:5" ht="18.75" customHeight="1">
-      <c r="A43" s="18"/>
-      <c r="B43" s="25"/>
+      <c r="A43" s="25"/>
+      <c r="B43" s="29"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
     </row>
     <row r="44" spans="1:5" ht="18.75" customHeight="1">
-      <c r="A44" s="18"/>
-      <c r="B44" s="24" t="s">
+      <c r="A44" s="25"/>
+      <c r="B44" s="28" t="s">
         <v>8</v>
       </c>
       <c r="C44" s="5"/>
@@ -6112,15 +6081,15 @@
       <c r="E44" s="5"/>
     </row>
     <row r="45" spans="1:5" ht="14.55" customHeight="1">
-      <c r="A45" s="18"/>
-      <c r="B45" s="25"/>
+      <c r="A45" s="25"/>
+      <c r="B45" s="29"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
     </row>
     <row r="46" spans="1:5" ht="16.05" customHeight="1">
-      <c r="A46" s="18"/>
-      <c r="B46" s="24" t="s">
+      <c r="A46" s="25"/>
+      <c r="B46" s="28" t="s">
         <v>10</v>
       </c>
       <c r="C46" s="5"/>
@@ -6128,71 +6097,71 @@
       <c r="E46" s="5"/>
     </row>
     <row r="47" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A47" s="19"/>
-      <c r="B47" s="25"/>
+      <c r="A47" s="15"/>
+      <c r="B47" s="29"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
     </row>
     <row r="48" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A48" s="17" t="s">
-        <v>77</v>
+      <c r="A48" s="14" t="s">
+        <v>75</v>
       </c>
       <c r="B48" s="20" t="s">
         <v>5</v>
       </c>
       <c r="C48" s="5"/>
-      <c r="D48" s="28" t="s">
-        <v>98</v>
+      <c r="D48" s="30" t="s">
+        <v>95</v>
       </c>
       <c r="E48" s="5"/>
     </row>
     <row r="49" spans="1:5" ht="40.799999999999997" customHeight="1">
-      <c r="A49" s="18"/>
+      <c r="A49" s="25"/>
       <c r="B49" s="21"/>
       <c r="C49" s="7"/>
-      <c r="D49" s="29"/>
+      <c r="D49" s="31"/>
       <c r="E49" s="7"/>
     </row>
     <row r="50" spans="1:5" ht="40.799999999999997" customHeight="1">
-      <c r="A50" s="18"/>
+      <c r="A50" s="25"/>
       <c r="B50" s="20" t="s">
         <v>6</v>
       </c>
       <c r="C50" s="7"/>
-      <c r="D50" s="28" t="s">
-        <v>98</v>
+      <c r="D50" s="30" t="s">
+        <v>95</v>
       </c>
       <c r="E50" s="7"/>
     </row>
     <row r="51" spans="1:5" ht="33" customHeight="1">
-      <c r="A51" s="18"/>
+      <c r="A51" s="25"/>
       <c r="B51" s="21"/>
       <c r="C51" s="7"/>
-      <c r="D51" s="29"/>
+      <c r="D51" s="31"/>
       <c r="E51" s="7"/>
     </row>
     <row r="52" spans="1:5" ht="28.05" customHeight="1">
-      <c r="A52" s="18"/>
-      <c r="B52" s="62" t="s">
+      <c r="A52" s="25"/>
+      <c r="B52" s="59" t="s">
         <v>8</v>
       </c>
       <c r="C52" s="7"/>
-      <c r="D52" s="28" t="s">
-        <v>99</v>
+      <c r="D52" s="30" t="s">
+        <v>96</v>
       </c>
       <c r="E52" s="7"/>
     </row>
     <row r="53" spans="1:5" ht="28.05" customHeight="1">
-      <c r="A53" s="18"/>
-      <c r="B53" s="63"/>
+      <c r="A53" s="25"/>
+      <c r="B53" s="60"/>
       <c r="C53" s="7"/>
-      <c r="D53" s="29"/>
+      <c r="D53" s="31"/>
       <c r="E53" s="7"/>
     </row>
     <row r="54" spans="1:5" ht="28.2" customHeight="1">
-      <c r="A54" s="18"/>
-      <c r="B54" s="62" t="s">
+      <c r="A54" s="25"/>
+      <c r="B54" s="59" t="s">
         <v>10</v>
       </c>
       <c r="C54" s="7"/>
@@ -6200,14 +6169,47 @@
       <c r="E54" s="7"/>
     </row>
     <row r="55" spans="1:5" ht="28.8" customHeight="1">
-      <c r="A55" s="19"/>
-      <c r="B55" s="63"/>
+      <c r="A55" s="15"/>
+      <c r="B55" s="60"/>
       <c r="C55" s="7"/>
       <c r="D55" s="7"/>
       <c r="E55" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="46">
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="A20:A29"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="A30:A39"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:D37"/>
+    <mergeCell ref="B38:B39"/>
     <mergeCell ref="B52:B53"/>
     <mergeCell ref="D52:D53"/>
     <mergeCell ref="B54:B55"/>
@@ -6221,39 +6223,6 @@
     <mergeCell ref="B50:B51"/>
     <mergeCell ref="D50:D51"/>
     <mergeCell ref="A48:A55"/>
-    <mergeCell ref="A30:A39"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:D37"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="A20:A29"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6286,8 +6255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -6301,74 +6270,74 @@
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17.7" customHeight="1">
-      <c r="A2" s="17" t="s">
-        <v>150</v>
+      <c r="A2" s="14" t="s">
+        <v>147</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="5"/>
-      <c r="D2" s="28" t="s">
-        <v>103</v>
+      <c r="D2" s="30" t="s">
+        <v>100</v>
       </c>
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" ht="16.05" customHeight="1">
-      <c r="A3" s="18"/>
+      <c r="A3" s="25"/>
       <c r="B3" s="21"/>
       <c r="C3" s="5"/>
-      <c r="D3" s="29"/>
+      <c r="D3" s="31"/>
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" ht="18.75" customHeight="1">
-      <c r="A4" s="18"/>
-      <c r="B4" s="24" t="s">
+      <c r="A4" s="25"/>
+      <c r="B4" s="28" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="D4" s="28" t="s">
-        <v>103</v>
+      <c r="D4" s="30" t="s">
+        <v>100</v>
       </c>
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A5" s="18"/>
-      <c r="B5" s="25"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="29"/>
       <c r="C5" s="5"/>
-      <c r="D5" s="29"/>
+      <c r="D5" s="31"/>
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A6" s="18"/>
-      <c r="B6" s="24" t="s">
+      <c r="A6" s="25"/>
+      <c r="B6" s="28" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="5"/>
-      <c r="D6" s="28" t="s">
-        <v>104</v>
+      <c r="D6" s="30" t="s">
+        <v>101</v>
       </c>
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A7" s="18"/>
-      <c r="B7" s="25"/>
+      <c r="A7" s="25"/>
+      <c r="B7" s="29"/>
       <c r="C7" s="5"/>
-      <c r="D7" s="29"/>
+      <c r="D7" s="31"/>
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" ht="11.25" customHeight="1">
-      <c r="A8" s="18"/>
-      <c r="B8" s="24" t="s">
+      <c r="A8" s="25"/>
+      <c r="B8" s="28" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="5"/>
@@ -6376,14 +6345,14 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="11.7" customHeight="1">
-      <c r="A9" s="19"/>
-      <c r="B9" s="25"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="29"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" ht="12" customHeight="1">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="14" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="20" t="s">
@@ -6394,107 +6363,107 @@
       <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:5" ht="10.95" customHeight="1">
-      <c r="A11" s="18"/>
+      <c r="A11" s="25"/>
       <c r="B11" s="21"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5" ht="33" customHeight="1">
-      <c r="A12" s="18"/>
-      <c r="B12" s="24" t="s">
+      <c r="A12" s="25"/>
+      <c r="B12" s="28" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:5" ht="33" customHeight="1">
-      <c r="A13" s="18"/>
-      <c r="B13" s="25"/>
+      <c r="A13" s="25"/>
+      <c r="B13" s="29"/>
       <c r="C13" s="7"/>
       <c r="D13" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:5" ht="18.75" customHeight="1">
-      <c r="A14" s="18"/>
-      <c r="B14" s="24" t="s">
+      <c r="A14" s="25"/>
+      <c r="B14" s="28" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="28" t="s">
-        <v>107</v>
+      <c r="D14" s="30" t="s">
+        <v>104</v>
       </c>
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" ht="18.75" customHeight="1">
-      <c r="A15" s="18"/>
-      <c r="B15" s="25"/>
+      <c r="A15" s="25"/>
+      <c r="B15" s="29"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="29"/>
+      <c r="D15" s="31"/>
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A16" s="18"/>
-      <c r="B16" s="24" t="s">
+      <c r="A16" s="25"/>
+      <c r="B16" s="28" t="s">
         <v>10</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
-      <c r="E16" s="28" t="s">
-        <v>107</v>
+      <c r="E16" s="30" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A17" s="18"/>
-      <c r="B17" s="25"/>
+      <c r="A17" s="25"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
-      <c r="E17" s="29"/>
+      <c r="E17" s="31"/>
     </row>
     <row r="18" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A18" s="18"/>
-      <c r="B18" s="24" t="s">
+      <c r="A18" s="25"/>
+      <c r="B18" s="28" t="s">
         <v>12</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
-      <c r="E18" s="28" t="s">
-        <v>108</v>
+      <c r="E18" s="30" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A19" s="18"/>
-      <c r="B19" s="25"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="29"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
-      <c r="E19" s="29"/>
+      <c r="E19" s="31"/>
     </row>
     <row r="20" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A20" s="18"/>
-      <c r="B20" s="24" t="s">
+      <c r="A20" s="25"/>
+      <c r="B20" s="28" t="s">
         <v>14</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
-      <c r="E20" s="28" t="s">
-        <v>109</v>
+      <c r="E20" s="30" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="17.7" customHeight="1">
-      <c r="A21" s="19"/>
-      <c r="B21" s="25"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="29"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
-      <c r="E21" s="29"/>
+      <c r="E21" s="31"/>
     </row>
     <row r="22" spans="1:5" ht="19.95" customHeight="1">
-      <c r="A22" s="30" t="s">
-        <v>28</v>
+      <c r="A22" s="38" t="s">
+        <v>27</v>
       </c>
       <c r="B22" s="20" t="s">
         <v>5</v>
@@ -6504,197 +6473,197 @@
       <c r="E22" s="5"/>
     </row>
     <row r="23" spans="1:5" ht="33" customHeight="1">
-      <c r="A23" s="31"/>
+      <c r="A23" s="39"/>
       <c r="B23" s="21"/>
       <c r="C23" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
     </row>
     <row r="24" spans="1:5" ht="33" customHeight="1">
-      <c r="A24" s="31"/>
-      <c r="B24" s="24" t="s">
+      <c r="A24" s="39"/>
+      <c r="B24" s="28" t="s">
         <v>6</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E24" s="7"/>
     </row>
     <row r="25" spans="1:5" ht="33" customHeight="1">
-      <c r="A25" s="31"/>
-      <c r="B25" s="25"/>
+      <c r="A25" s="39"/>
+      <c r="B25" s="29"/>
       <c r="C25" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
     </row>
     <row r="26" spans="1:5" ht="33" customHeight="1">
-      <c r="A26" s="31"/>
-      <c r="B26" s="24" t="s">
+      <c r="A26" s="39"/>
+      <c r="B26" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="28" t="s">
-        <v>114</v>
+      <c r="C26" s="30" t="s">
+        <v>111</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="33" customHeight="1">
-      <c r="A27" s="31"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="29"/>
+      <c r="A27" s="39"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="31"/>
       <c r="D27" s="7"/>
       <c r="E27" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="33" customHeight="1">
+      <c r="A28" s="39"/>
+      <c r="B28" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E28" s="30" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="33" customHeight="1">
+      <c r="A29" s="39"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="33" customHeight="1">
-      <c r="A28" s="31"/>
-      <c r="B28" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E28" s="28" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="33" customHeight="1">
-      <c r="A29" s="31"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="2" t="s">
-        <v>119</v>
-      </c>
       <c r="D29" s="7"/>
-      <c r="E29" s="29"/>
+      <c r="E29" s="31"/>
     </row>
     <row r="30" spans="1:5" ht="33" customHeight="1">
-      <c r="A30" s="31"/>
-      <c r="B30" s="24" t="s">
+      <c r="A30" s="39"/>
+      <c r="B30" s="28" t="s">
         <v>12</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D30" s="7"/>
-      <c r="E30" s="28" t="s">
-        <v>108</v>
+      <c r="E30" s="30" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="17.7" customHeight="1">
-      <c r="A31" s="32"/>
-      <c r="B31" s="25"/>
+      <c r="A31" s="40"/>
+      <c r="B31" s="29"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
-      <c r="E31" s="29"/>
+      <c r="E31" s="31"/>
     </row>
     <row r="32" spans="1:5" ht="19.95" customHeight="1">
-      <c r="A32" s="30" t="s">
-        <v>43</v>
+      <c r="A32" s="38" t="s">
+        <v>41</v>
       </c>
       <c r="B32" s="20" t="s">
         <v>5</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
-      <c r="E32" s="28" t="s">
-        <v>120</v>
+      <c r="E32" s="30" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="33" customHeight="1">
-      <c r="A33" s="31"/>
+      <c r="A33" s="39"/>
       <c r="B33" s="21"/>
       <c r="C33" s="7"/>
       <c r="D33" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E33" s="29"/>
+        <v>118</v>
+      </c>
+      <c r="E33" s="31"/>
     </row>
     <row r="34" spans="1:5" ht="33" customHeight="1">
-      <c r="A34" s="31"/>
-      <c r="B34" s="24" t="s">
+      <c r="A34" s="39"/>
+      <c r="B34" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C34" s="28" t="s">
-        <v>122</v>
+      <c r="C34" s="30" t="s">
+        <v>119</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E34" s="28" t="s">
-        <v>115</v>
+        <v>100</v>
+      </c>
+      <c r="E34" s="30" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="33" customHeight="1">
-      <c r="A35" s="31"/>
-      <c r="B35" s="25"/>
-      <c r="C35" s="29"/>
+      <c r="A35" s="39"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="31"/>
       <c r="D35" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E35" s="29"/>
+        <v>118</v>
+      </c>
+      <c r="E35" s="31"/>
     </row>
     <row r="36" spans="1:5" ht="35.549999999999997" customHeight="1">
-      <c r="A36" s="31"/>
+      <c r="A36" s="39"/>
       <c r="B36" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="20.25" customHeight="1">
-      <c r="A37" s="31"/>
+      <c r="A37" s="39"/>
       <c r="B37" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C37" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="D37" s="46"/>
-      <c r="E37" s="47"/>
+      <c r="C37" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37" s="23"/>
+      <c r="E37" s="24"/>
     </row>
     <row r="38" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A38" s="31"/>
-      <c r="B38" s="24" t="s">
+      <c r="A38" s="39"/>
+      <c r="B38" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C38" s="28" t="s">
-        <v>125</v>
+      <c r="C38" s="30" t="s">
+        <v>122</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
     </row>
     <row r="39" spans="1:5" ht="16.95" customHeight="1">
-      <c r="A39" s="31"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="29"/>
+      <c r="A39" s="39"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="31"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
     </row>
     <row r="40" spans="1:5" ht="10.95" customHeight="1">
-      <c r="A40" s="31"/>
-      <c r="B40" s="24" t="s">
+      <c r="A40" s="39"/>
+      <c r="B40" s="28" t="s">
         <v>14</v>
       </c>
       <c r="C40" s="5"/>
@@ -6702,108 +6671,108 @@
       <c r="E40" s="5"/>
     </row>
     <row r="41" spans="1:5" ht="11.7" customHeight="1">
-      <c r="A41" s="32"/>
-      <c r="B41" s="25"/>
+      <c r="A41" s="40"/>
+      <c r="B41" s="29"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
     </row>
     <row r="42" spans="1:5" ht="33" customHeight="1">
-      <c r="A42" s="17" t="s">
-        <v>54</v>
+      <c r="A42" s="14" t="s">
+        <v>52</v>
       </c>
       <c r="B42" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="28" t="s">
-        <v>126</v>
+      <c r="C42" s="30" t="s">
+        <v>123</v>
       </c>
       <c r="D42" s="7"/>
       <c r="E42" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="33" customHeight="1">
-      <c r="A43" s="18"/>
+      <c r="A43" s="25"/>
       <c r="B43" s="21"/>
-      <c r="C43" s="29"/>
+      <c r="C43" s="31"/>
       <c r="D43" s="7"/>
       <c r="E43" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="33" customHeight="1">
-      <c r="A44" s="18"/>
+      <c r="A44" s="25"/>
       <c r="B44" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C44" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="33" customHeight="1">
+      <c r="A45" s="25"/>
+      <c r="B45" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D45" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="E45" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="33" customHeight="1">
-      <c r="A45" s="18"/>
-      <c r="B45" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="C45" s="28" t="s">
-        <v>132</v>
-      </c>
-      <c r="D45" s="28" t="s">
-        <v>133</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
     <row r="46" spans="1:5" ht="33" customHeight="1">
-      <c r="A46" s="18"/>
-      <c r="B46" s="25"/>
-      <c r="C46" s="29"/>
-      <c r="D46" s="29"/>
+      <c r="A46" s="25"/>
+      <c r="B46" s="29"/>
+      <c r="C46" s="31"/>
+      <c r="D46" s="31"/>
       <c r="E46" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="16.2" customHeight="1">
-      <c r="A47" s="18"/>
-      <c r="B47" s="24" t="s">
+      <c r="A47" s="25"/>
+      <c r="B47" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C47" s="28" t="s">
-        <v>132</v>
+      <c r="C47" s="30" t="s">
+        <v>129</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
     </row>
     <row r="48" spans="1:5" ht="16.8" customHeight="1">
-      <c r="A48" s="19"/>
-      <c r="B48" s="25"/>
-      <c r="C48" s="29"/>
+      <c r="A48" s="15"/>
+      <c r="B48" s="29"/>
+      <c r="C48" s="31"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
     </row>
     <row r="49" spans="1:5" ht="17.7" customHeight="1">
-      <c r="A49" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="B49" s="13" t="s">
-        <v>59</v>
+      <c r="A49" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
     </row>
     <row r="50" spans="1:5" ht="25.5" customHeight="1">
-      <c r="A50" s="19"/>
-      <c r="B50" s="13" t="s">
-        <v>60</v>
+      <c r="A50" s="15"/>
+      <c r="B50" s="12" t="s">
+        <v>58</v>
       </c>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
@@ -6811,15 +6780,28 @@
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="A42:A48"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A10:A21"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="E28:E29"/>
     <mergeCell ref="B30:B31"/>
     <mergeCell ref="E30:E31"/>
     <mergeCell ref="A32:A41"/>
@@ -6836,28 +6818,15 @@
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="A10:A21"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A42:A48"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>